<commit_message>
Download or sent statement to email fully implemented in History Page
</commit_message>
<xml_diff>
--- a/Backend/src/api/controllers/statement_80003.xlsx
+++ b/Backend/src/api/controllers/statement_80003.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -28,16 +28,40 @@
     <t>Description</t>
   </si>
   <si>
+    <t>Canceled</t>
+  </si>
+  <si>
     <t>2024-05-14</t>
   </si>
   <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
     <t>Food on campussssss</t>
   </si>
   <si>
-    <t>2024-05-30</t>
-  </si>
-  <si>
-    <t>Essay for friend</t>
+    <t>No</t>
+  </si>
+  <si>
+    <t>2024-05-15</t>
+  </si>
+  <si>
+    <t>Writing essays</t>
+  </si>
+  <si>
+    <t>Essay for friend 6</t>
+  </si>
+  <si>
+    <t>2024-06-01</t>
+  </si>
+  <si>
+    <t>Pizza</t>
+  </si>
+  <si>
+    <t>Essay for friend3</t>
   </si>
 </sst>
 </file>
@@ -90,6 +114,28 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="TransactionTable" displayName="TransactionTable" ref="A1:F5" totalsRowShown="1" headerRowCount="1">
+  <autoFilter ref="A1:F5">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Date" totalsRowLabel="Total"/>
+    <tableColumn id="2" name="Type" totalsRowFunction="none"/>
+    <tableColumn id="3" name="Amount" totalsRowFunction="none"/>
+    <tableColumn id="4" name="Category" totalsRowFunction="none"/>
+    <tableColumn id="5" name="Description" totalsRowFunction="none"/>
+    <tableColumn id="6" name="Canceled" totalsRowFunction="none"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -414,16 +460,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="3" width="10" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="30" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -439,31 +486,95 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
       </c>
       <c r="C2">
         <v>100</v>
       </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3">
-        <v>3000</v>
+        <v>44</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
       </c>
       <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>70</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Improved style for History Page
</commit_message>
<xml_diff>
--- a/Backend/src/api/controllers/statement_80003.xlsx
+++ b/Backend/src/api/controllers/statement_80003.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>Essay for friend 6</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
   <si>
     <t>2024-06-01</t>
@@ -527,12 +530,12 @@
         <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -544,7 +547,7 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
@@ -552,7 +555,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -564,7 +567,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>

</xml_diff>